<commit_message>
feat(ai): add ai-service core and backend integration
</commit_message>
<xml_diff>
--- a/server/utils/Sample_Students.xlsx
+++ b/server/utils/Sample_Students.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\SIH-MarkME\server\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CC13BDC-55B1-495C-80FF-828C5844B55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011DB52A-E260-40FD-AF57-6E41FAC2C4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -52,26 +52,50 @@
     <t>2008-08-18</t>
   </si>
   <si>
-    <t>Elon Musk</t>
-  </si>
-  <si>
-    <t>Jeff Bezoz</t>
-  </si>
-  <si>
-    <t>Satya Nandela</t>
-  </si>
-  <si>
-    <t>Sundar Pichai</t>
-  </si>
-  <si>
-    <t>Bill Gates</t>
+    <t>Vedant</t>
+  </si>
+  <si>
+    <t>Kartik</t>
+  </si>
+  <si>
+    <t>Aryan</t>
+  </si>
+  <si>
+    <t>Krish</t>
+  </si>
+  <si>
+    <t>Vraj</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Mohan</t>
+  </si>
+  <si>
+    <t>Sohan</t>
+  </si>
+  <si>
+    <t>Shivam</t>
+  </si>
+  <si>
+    <t>2008-08-19</t>
+  </si>
+  <si>
+    <t>2008-08-20</t>
+  </si>
+  <si>
+    <t>2008-08-21</t>
+  </si>
+  <si>
+    <t>2008-08-22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,16 +103,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -96,13 +156,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -407,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -435,76 +522,133 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>101</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>102</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
+        <v>103</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4">
         <v>104</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1">
-        <v>103</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>105</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4">
+        <v>106</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4">
+        <v>107</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4">
+        <v>108</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4">
+        <v>109</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>